<commit_message>
add raven and coding
</commit_message>
<xml_diff>
--- a/reports/model_space_new/docs/domains-naming-map.xlsx
+++ b/reports/model_space_new/docs/domains-naming-map.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\koval_000\Documents\GitHub\IALSA-2015-Portland\reports\model_space_new\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\piccinin\Documents\GitHub\IALSA-2015-Portland\reports\model_space_new\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="118">
   <si>
     <t>Digitsymbolsubstitution=symbol</t>
   </si>
@@ -397,6 +397,12 @@
   </si>
   <si>
     <t>digitsbackward</t>
+  </si>
+  <si>
+    <t xml:space="preserve">raven     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">codingtask     </t>
   </si>
 </sst>
 </file>
@@ -441,12 +447,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="8">
@@ -546,7 +558,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -560,23 +572,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -587,9 +596,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -876,14 +889,14 @@
       <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.5546875" customWidth="1"/>
-    <col min="2" max="2" width="46.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.54296875" customWidth="1"/>
+    <col min="2" max="2" width="46.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -894,7 +907,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>66</v>
       </c>
@@ -905,7 +918,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>66</v>
       </c>
@@ -913,7 +926,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>66</v>
       </c>
@@ -921,7 +934,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="43.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>66</v>
       </c>
@@ -929,7 +942,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="29.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>66</v>
       </c>
@@ -937,7 +950,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>67</v>
       </c>
@@ -948,7 +961,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -959,7 +972,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -967,7 +980,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -978,7 +991,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>27</v>
       </c>
@@ -986,7 +999,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>27</v>
       </c>
@@ -994,7 +1007,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>27</v>
       </c>
@@ -1002,7 +1015,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="100.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" ht="100.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -1010,7 +1023,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>27</v>
       </c>
@@ -1018,7 +1031,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>27</v>
       </c>
@@ -1026,7 +1039,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -1034,7 +1047,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>27</v>
       </c>
@@ -1042,7 +1055,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" ht="29.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>27</v>
       </c>
@@ -1050,7 +1063,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>39</v>
       </c>
@@ -1061,7 +1074,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" ht="43.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>39</v>
       </c>
@@ -1069,7 +1082,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>39</v>
       </c>
@@ -1077,7 +1090,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" ht="28.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>44</v>
       </c>
@@ -1088,7 +1101,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>47</v>
       </c>
@@ -1099,7 +1112,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>47</v>
       </c>
@@ -1107,7 +1120,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="86.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" ht="86.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>48</v>
       </c>
@@ -1115,12 +1128,12 @@
         <v>52</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B32" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>54</v>
       </c>
@@ -1131,17 +1144,17 @@
         <v>55</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" ht="43.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B35" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="43.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" ht="43.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B36" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>59</v>
       </c>
@@ -1152,27 +1165,27 @@
         <v>60</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B38" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" ht="43.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B39" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" ht="43.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B40" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B41" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>61</v>
       </c>
@@ -1183,27 +1196,27 @@
         <v>62</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B43" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B44" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B45" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B46" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>65</v>
       </c>
@@ -1216,23 +1229,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F46"/>
+  <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29:A35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.75" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="25" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" customWidth="1"/>
-    <col min="3" max="3" width="24.44140625" customWidth="1"/>
-    <col min="4" max="4" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.453125" customWidth="1"/>
+    <col min="3" max="3" width="24.453125" customWidth="1"/>
+    <col min="4" max="4" width="19.6328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="13.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="13.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -1242,21 +1255,21 @@
       <c r="C1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="6" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="7" t="s">
         <v>14</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -1266,9 +1279,9 @@
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
+    <row r="3" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="8"/>
+      <c r="B3" s="8"/>
       <c r="C3" s="3" t="s">
         <v>16</v>
       </c>
@@ -1276,9 +1289,9 @@
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
+    <row r="4" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="8"/>
+      <c r="B4" s="8"/>
       <c r="C4" s="3" t="s">
         <v>17</v>
       </c>
@@ -1286,9 +1299,9 @@
         <v>71</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
+    <row r="5" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="8"/>
+      <c r="B5" s="8"/>
       <c r="C5" s="3" t="s">
         <v>18</v>
       </c>
@@ -1299,9 +1312,9 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="13.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
+    <row r="6" spans="1:6" ht="13.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="9"/>
+      <c r="B6" s="9"/>
       <c r="C6" s="4" t="s">
         <v>19</v>
       </c>
@@ -1309,14 +1322,14 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="6" t="s">
+    <row r="7" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="13" t="s">
         <v>22</v>
       </c>
       <c r="D7" t="s">
@@ -1326,16 +1339,16 @@
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="13.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="9"/>
-    </row>
-    <row r="9" spans="1:6" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="6" t="s">
+    <row r="8" spans="1:6" ht="13.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="9"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="14"/>
+    </row>
+    <row r="9" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="7" t="s">
         <v>24</v>
       </c>
       <c r="C9" s="3" t="s">
@@ -1345,9 +1358,9 @@
         <v>76</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
+    <row r="10" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="8"/>
+      <c r="B10" s="8"/>
       <c r="C10" s="3" t="s">
         <v>26</v>
       </c>
@@ -1358,16 +1371,16 @@
         <v>78</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="13.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="7"/>
-      <c r="B11" s="7"/>
+    <row r="11" spans="1:6" ht="13.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="9"/>
+      <c r="B11" s="9"/>
       <c r="C11" s="4"/>
     </row>
-    <row r="12" spans="1:6" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="6" t="s">
+    <row r="12" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="7" t="s">
         <v>28</v>
       </c>
       <c r="C12" s="3" t="s">
@@ -1377,9 +1390,9 @@
         <v>79</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
+    <row r="13" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="8"/>
+      <c r="B13" s="8"/>
       <c r="C13" s="3" t="s">
         <v>30</v>
       </c>
@@ -1387,9 +1400,9 @@
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
+    <row r="14" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="8"/>
+      <c r="B14" s="8"/>
       <c r="C14" s="3" t="s">
         <v>31</v>
       </c>
@@ -1397,9 +1410,9 @@
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5"/>
+    <row r="15" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="8"/>
+      <c r="B15" s="8"/>
       <c r="C15" s="3" t="s">
         <v>32</v>
       </c>
@@ -1407,9 +1420,9 @@
         <v>82</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
+    <row r="16" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="8"/>
+      <c r="B16" s="8"/>
       <c r="C16" s="3" t="s">
         <v>33</v>
       </c>
@@ -1417,9 +1430,9 @@
         <v>83</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5"/>
+    <row r="17" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="8"/>
+      <c r="B17" s="8"/>
       <c r="C17" s="3" t="s">
         <v>34</v>
       </c>
@@ -1427,9 +1440,9 @@
         <v>84</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
+    <row r="18" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="8"/>
+      <c r="B18" s="8"/>
       <c r="C18" s="3" t="s">
         <v>35</v>
       </c>
@@ -1437,9 +1450,9 @@
         <v>85</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="5"/>
-      <c r="B19" s="5"/>
+    <row r="19" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="8"/>
+      <c r="B19" s="8"/>
       <c r="C19" s="3" t="s">
         <v>36</v>
       </c>
@@ -1447,9 +1460,9 @@
         <v>86</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="5"/>
-      <c r="B20" s="5"/>
+    <row r="20" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="8"/>
+      <c r="B20" s="8"/>
       <c r="C20" s="3" t="s">
         <v>37</v>
       </c>
@@ -1457,9 +1470,9 @@
         <v>87</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="13.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="7"/>
-      <c r="B21" s="7"/>
+    <row r="21" spans="1:6" ht="13.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="9"/>
+      <c r="B21" s="9"/>
       <c r="C21" s="4" t="s">
         <v>38</v>
       </c>
@@ -1467,11 +1480,11 @@
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="6" t="s">
+    <row r="22" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="7" t="s">
         <v>40</v>
       </c>
       <c r="C22" s="3" t="s">
@@ -1487,16 +1500,16 @@
         <v>89</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="5"/>
-      <c r="B23" s="5"/>
+    <row r="23" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="8"/>
+      <c r="B23" s="8"/>
       <c r="C23" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="5"/>
-      <c r="B24" s="5"/>
+    <row r="24" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="8"/>
+      <c r="B24" s="8"/>
       <c r="C24" s="3" t="s">
         <v>43</v>
       </c>
@@ -1504,40 +1517,40 @@
         <v>93</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="5"/>
-      <c r="B25" s="5"/>
+    <row r="25" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="8"/>
+      <c r="B25" s="8"/>
       <c r="C25" s="3"/>
     </row>
-    <row r="26" spans="1:6" ht="13.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="7"/>
-      <c r="B26" s="7"/>
+    <row r="26" spans="1:6" ht="13.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A26" s="9"/>
+      <c r="B26" s="9"/>
       <c r="C26" s="4"/>
     </row>
-    <row r="27" spans="1:6" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="6" t="s">
+    <row r="27" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B27" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="C27" s="8" t="s">
+      <c r="C27" s="13" t="s">
         <v>46</v>
       </c>
       <c r="D27" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="13.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="7"/>
-      <c r="B28" s="7"/>
-      <c r="C28" s="9"/>
-    </row>
-    <row r="29" spans="1:6" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="11" t="s">
+    <row r="28" spans="1:6" ht="13.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A28" s="9"/>
+      <c r="B28" s="9"/>
+      <c r="C28" s="14"/>
+    </row>
+    <row r="29" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="B29" s="7" t="s">
         <v>49</v>
       </c>
       <c r="C29" s="3" t="s">
@@ -1550,9 +1563,9 @@
         <v>95</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="12"/>
-      <c r="B30" s="5"/>
+    <row r="30" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="11"/>
+      <c r="B30" s="8"/>
       <c r="C30" s="3" t="s">
         <v>51</v>
       </c>
@@ -1560,19 +1573,22 @@
         <v>96</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="12"/>
-      <c r="B31" s="5"/>
+    <row r="31" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="11"/>
+      <c r="B31" s="8"/>
       <c r="C31" s="3" t="s">
         <v>52</v>
       </c>
       <c r="D31" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="12"/>
-      <c r="B32" s="5"/>
+      <c r="E31" s="15" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="11"/>
+      <c r="B32" s="8"/>
       <c r="C32" s="3" t="s">
         <v>53</v>
       </c>
@@ -1580,9 +1596,9 @@
         <v>98</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="12"/>
-      <c r="B33" s="5"/>
+    <row r="33" spans="1:7" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="11"/>
+      <c r="B33" s="8"/>
       <c r="C33" s="3" t="s">
         <v>56</v>
       </c>
@@ -1593,9 +1609,9 @@
         <v>100</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="12"/>
-      <c r="B34" s="5"/>
+    <row r="34" spans="1:7" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="11"/>
+      <c r="B34" s="8"/>
       <c r="C34" s="3" t="s">
         <v>57</v>
       </c>
@@ -1603,9 +1619,9 @@
         <v>57</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="13.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="13"/>
-      <c r="B35" s="7"/>
+    <row r="35" spans="1:7" ht="13.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A35" s="12"/>
+      <c r="B35" s="9"/>
       <c r="C35" s="4" t="s">
         <v>58</v>
       </c>
@@ -1616,11 +1632,11 @@
         <v>102</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="6" t="s">
+    <row r="36" spans="1:7" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="B36" s="6" t="s">
+      <c r="B36" s="7" t="s">
         <v>60</v>
       </c>
       <c r="C36" s="3" t="s">
@@ -1635,10 +1651,13 @@
       <c r="F36" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="5"/>
-      <c r="B37" s="5"/>
+      <c r="G36" s="15" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="8"/>
+      <c r="B37" s="8"/>
       <c r="C37" s="3" t="s">
         <v>1</v>
       </c>
@@ -1646,9 +1665,9 @@
         <v>106</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="5"/>
-      <c r="B38" s="5"/>
+    <row r="38" spans="1:7" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="8"/>
+      <c r="B38" s="8"/>
       <c r="C38" s="3" t="s">
         <v>2</v>
       </c>
@@ -1659,9 +1678,9 @@
         <v>108</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="5"/>
-      <c r="B39" s="5"/>
+    <row r="39" spans="1:7" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="8"/>
+      <c r="B39" s="8"/>
       <c r="C39" s="3" t="s">
         <v>3</v>
       </c>
@@ -1672,9 +1691,9 @@
         <v>110</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="13.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="7"/>
-      <c r="B40" s="7"/>
+    <row r="40" spans="1:7" ht="13.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A40" s="9"/>
+      <c r="B40" s="9"/>
       <c r="C40" s="4" t="s">
         <v>4</v>
       </c>
@@ -1682,11 +1701,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="6" t="s">
+    <row r="41" spans="1:7" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="B41" s="6" t="s">
+      <c r="B41" s="7" t="s">
         <v>62</v>
       </c>
       <c r="C41" s="3" t="s">
@@ -1699,9 +1718,9 @@
         <v>111</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="5"/>
-      <c r="B42" s="5"/>
+    <row r="42" spans="1:7" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="8"/>
+      <c r="B42" s="8"/>
       <c r="C42" s="3" t="s">
         <v>6</v>
       </c>
@@ -1709,9 +1728,9 @@
         <v>112</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="5"/>
-      <c r="B43" s="5"/>
+    <row r="43" spans="1:7" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="8"/>
+      <c r="B43" s="8"/>
       <c r="C43" s="3" t="s">
         <v>7</v>
       </c>
@@ -1719,9 +1738,9 @@
         <v>113</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="5"/>
-      <c r="B44" s="5"/>
+    <row r="44" spans="1:7" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="8"/>
+      <c r="B44" s="8"/>
       <c r="C44" s="3" t="s">
         <v>8</v>
       </c>
@@ -1729,9 +1748,9 @@
         <v>114</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="13.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="7"/>
-      <c r="B45" s="7"/>
+    <row r="45" spans="1:7" ht="13.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A45" s="9"/>
+      <c r="B45" s="9"/>
       <c r="C45" s="4" t="s">
         <v>9</v>
       </c>
@@ -1739,13 +1758,19 @@
         <v>9</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="10" t="s">
+    <row r="46" spans="1:7" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="5" t="s">
         <v>63</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="B2:B6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="B9:B11"/>
     <mergeCell ref="A41:A45"/>
     <mergeCell ref="B41:B45"/>
     <mergeCell ref="A29:A35"/>
@@ -1760,13 +1785,8 @@
     <mergeCell ref="B22:B26"/>
     <mergeCell ref="A27:A28"/>
     <mergeCell ref="B27:B28"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="B2:B6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="B9:B11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Revert "office wrong turn"
This reverts commit 324b4a0f2696a490d61aea4ce86789070caf8bc9.
</commit_message>
<xml_diff>
--- a/reports/model_space_new/docs/domains-naming-map.xlsx
+++ b/reports/model_space_new/docs/domains-naming-map.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andkov\Documents\GitHub\IALSA-2015-Portland\reports\model_space_new\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\piccinin\Documents\GitHub\IALSA-2015-Portland\reports\model_space_new\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -351,6 +351,9 @@
     <t>lpsspatialability</t>
   </si>
   <si>
+    <t>ipsspatialability</t>
+  </si>
+  <si>
     <t>line</t>
   </si>
   <si>
@@ -400,9 +403,6 @@
   </si>
   <si>
     <t xml:space="preserve">codingtask     </t>
-  </si>
-  <si>
-    <t>lpsspacialability</t>
   </si>
 </sst>
 </file>
@@ -578,7 +578,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -603,6 +602,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -889,14 +889,14 @@
       <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" customWidth="1"/>
-    <col min="2" max="2" width="46.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.54296875" customWidth="1"/>
+    <col min="2" max="2" width="46.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -907,7 +907,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>66</v>
       </c>
@@ -918,7 +918,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>66</v>
       </c>
@@ -926,7 +926,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="28.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>66</v>
       </c>
@@ -934,7 +934,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="43.35" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="43.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>66</v>
       </c>
@@ -942,7 +942,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="29.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>66</v>
       </c>
@@ -950,7 +950,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>67</v>
       </c>
@@ -961,7 +961,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -972,7 +972,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="28.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -980,7 +980,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -991,7 +991,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="28.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>27</v>
       </c>
@@ -999,7 +999,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="28.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>27</v>
       </c>
@@ -1007,7 +1007,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="28.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>27</v>
       </c>
@@ -1015,7 +1015,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="100.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="100.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -1023,7 +1023,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="28.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>27</v>
       </c>
@@ -1031,7 +1031,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="28.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>27</v>
       </c>
@@ -1039,7 +1039,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="28.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -1047,7 +1047,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>27</v>
       </c>
@@ -1055,7 +1055,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="29.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>27</v>
       </c>
@@ -1063,7 +1063,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>39</v>
       </c>
@@ -1074,7 +1074,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="43.35" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="43.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>39</v>
       </c>
@@ -1082,7 +1082,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="28.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>39</v>
       </c>
@@ -1090,7 +1090,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="28.35" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="28.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>44</v>
       </c>
@@ -1101,7 +1101,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>47</v>
       </c>
@@ -1112,7 +1112,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="28.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>47</v>
       </c>
@@ -1120,7 +1120,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="86.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" ht="86.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>48</v>
       </c>
@@ -1128,12 +1128,12 @@
         <v>52</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B32" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>54</v>
       </c>
@@ -1144,17 +1144,17 @@
         <v>55</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="43.35" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" ht="43.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B35" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="43.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" ht="43.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B36" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>59</v>
       </c>
@@ -1165,27 +1165,27 @@
         <v>60</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B38" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="43.35" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" ht="43.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B39" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="43.35" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" ht="43.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B40" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B41" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>61</v>
       </c>
@@ -1196,27 +1196,27 @@
         <v>62</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B43" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B44" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B45" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B46" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>65</v>
       </c>
@@ -1232,21 +1232,20 @@
   <dimension ref="A1:G46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+      <selection activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.7" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.75" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.140625" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25" customWidth="1"/>
+    <col min="2" max="2" width="9.453125" customWidth="1"/>
+    <col min="3" max="3" width="24.453125" customWidth="1"/>
+    <col min="4" max="4" width="19.6328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="13.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="13.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -1266,11 +1265,11 @@
         <v>92</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>14</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -1280,9 +1279,9 @@
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="9"/>
-      <c r="B3" s="9"/>
+    <row r="3" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="8"/>
+      <c r="B3" s="8"/>
       <c r="C3" s="3" t="s">
         <v>16</v>
       </c>
@@ -1290,9 +1289,9 @@
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="9"/>
-      <c r="B4" s="9"/>
+    <row r="4" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="8"/>
+      <c r="B4" s="8"/>
       <c r="C4" s="3" t="s">
         <v>17</v>
       </c>
@@ -1300,9 +1299,9 @@
         <v>71</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="9"/>
-      <c r="B5" s="9"/>
+    <row r="5" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="8"/>
+      <c r="B5" s="8"/>
       <c r="C5" s="3" t="s">
         <v>18</v>
       </c>
@@ -1313,9 +1312,9 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="13.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="10"/>
-      <c r="B6" s="10"/>
+    <row r="6" spans="1:6" ht="13.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="9"/>
+      <c r="B6" s="9"/>
       <c r="C6" s="4" t="s">
         <v>19</v>
       </c>
@@ -1323,14 +1322,14 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+    <row r="7" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="13" t="s">
         <v>22</v>
       </c>
       <c r="D7" t="s">
@@ -1340,16 +1339,16 @@
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="13.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="10"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="15"/>
-    </row>
-    <row r="9" spans="1:6" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+    <row r="8" spans="1:6" ht="13.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="9"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="14"/>
+    </row>
+    <row r="9" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="7" t="s">
         <v>24</v>
       </c>
       <c r="C9" s="3" t="s">
@@ -1359,9 +1358,9 @@
         <v>76</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="9"/>
-      <c r="B10" s="9"/>
+    <row r="10" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="8"/>
+      <c r="B10" s="8"/>
       <c r="C10" s="3" t="s">
         <v>26</v>
       </c>
@@ -1372,16 +1371,16 @@
         <v>78</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="13.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="10"/>
-      <c r="B11" s="10"/>
+    <row r="11" spans="1:6" ht="13.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="9"/>
+      <c r="B11" s="9"/>
       <c r="C11" s="4"/>
     </row>
-    <row r="12" spans="1:6" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
+    <row r="12" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="7" t="s">
         <v>28</v>
       </c>
       <c r="C12" s="3" t="s">
@@ -1391,9 +1390,9 @@
         <v>79</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="9"/>
-      <c r="B13" s="9"/>
+    <row r="13" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="8"/>
+      <c r="B13" s="8"/>
       <c r="C13" s="3" t="s">
         <v>30</v>
       </c>
@@ -1401,9 +1400,9 @@
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="9"/>
-      <c r="B14" s="9"/>
+    <row r="14" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="8"/>
+      <c r="B14" s="8"/>
       <c r="C14" s="3" t="s">
         <v>31</v>
       </c>
@@ -1411,9 +1410,9 @@
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="9"/>
-      <c r="B15" s="9"/>
+    <row r="15" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="8"/>
+      <c r="B15" s="8"/>
       <c r="C15" s="3" t="s">
         <v>32</v>
       </c>
@@ -1421,9 +1420,9 @@
         <v>82</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="9"/>
-      <c r="B16" s="9"/>
+    <row r="16" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="8"/>
+      <c r="B16" s="8"/>
       <c r="C16" s="3" t="s">
         <v>33</v>
       </c>
@@ -1431,9 +1430,9 @@
         <v>83</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="9"/>
-      <c r="B17" s="9"/>
+    <row r="17" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="8"/>
+      <c r="B17" s="8"/>
       <c r="C17" s="3" t="s">
         <v>34</v>
       </c>
@@ -1441,9 +1440,9 @@
         <v>84</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="9"/>
-      <c r="B18" s="9"/>
+    <row r="18" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="8"/>
+      <c r="B18" s="8"/>
       <c r="C18" s="3" t="s">
         <v>35</v>
       </c>
@@ -1451,9 +1450,9 @@
         <v>85</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="9"/>
-      <c r="B19" s="9"/>
+    <row r="19" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="8"/>
+      <c r="B19" s="8"/>
       <c r="C19" s="3" t="s">
         <v>36</v>
       </c>
@@ -1461,9 +1460,9 @@
         <v>86</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="9"/>
-      <c r="B20" s="9"/>
+    <row r="20" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="8"/>
+      <c r="B20" s="8"/>
       <c r="C20" s="3" t="s">
         <v>37</v>
       </c>
@@ -1471,9 +1470,9 @@
         <v>87</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="13.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="10"/>
-      <c r="B21" s="10"/>
+    <row r="21" spans="1:6" ht="13.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="9"/>
+      <c r="B21" s="9"/>
       <c r="C21" s="4" t="s">
         <v>38</v>
       </c>
@@ -1481,18 +1480,18 @@
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="8" t="s">
+    <row r="22" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="B22" s="8" t="s">
+      <c r="B22" s="7" t="s">
         <v>40</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>41</v>
       </c>
       <c r="D22" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E22" t="s">
         <v>88</v>
@@ -1501,16 +1500,16 @@
         <v>89</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="9"/>
-      <c r="B23" s="9"/>
+    <row r="23" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="8"/>
+      <c r="B23" s="8"/>
       <c r="C23" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="9"/>
-      <c r="B24" s="9"/>
+    <row r="24" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="8"/>
+      <c r="B24" s="8"/>
       <c r="C24" s="3" t="s">
         <v>43</v>
       </c>
@@ -1518,40 +1517,40 @@
         <v>93</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="9"/>
-      <c r="B25" s="9"/>
+    <row r="25" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="8"/>
+      <c r="B25" s="8"/>
       <c r="C25" s="3"/>
     </row>
-    <row r="26" spans="1:6" ht="13.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="10"/>
-      <c r="B26" s="10"/>
+    <row r="26" spans="1:6" ht="13.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A26" s="9"/>
+      <c r="B26" s="9"/>
       <c r="C26" s="4"/>
     </row>
-    <row r="27" spans="1:6" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="8" t="s">
+    <row r="27" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B27" s="8" t="s">
+      <c r="B27" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="C27" s="14" t="s">
+      <c r="C27" s="13" t="s">
         <v>46</v>
       </c>
       <c r="D27" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="13.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="10"/>
-      <c r="B28" s="10"/>
-      <c r="C28" s="15"/>
-    </row>
-    <row r="29" spans="1:6" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="11" t="s">
+    <row r="28" spans="1:6" ht="13.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A28" s="9"/>
+      <c r="B28" s="9"/>
+      <c r="C28" s="14"/>
+    </row>
+    <row r="29" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="B29" s="8" t="s">
+      <c r="B29" s="7" t="s">
         <v>49</v>
       </c>
       <c r="C29" s="3" t="s">
@@ -1564,9 +1563,9 @@
         <v>95</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="12"/>
-      <c r="B30" s="9"/>
+    <row r="30" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="11"/>
+      <c r="B30" s="8"/>
       <c r="C30" s="3" t="s">
         <v>51</v>
       </c>
@@ -1574,22 +1573,22 @@
         <v>96</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="12"/>
-      <c r="B31" s="9"/>
+    <row r="31" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="11"/>
+      <c r="B31" s="8"/>
       <c r="C31" s="3" t="s">
         <v>52</v>
       </c>
       <c r="D31" t="s">
         <v>97</v>
       </c>
-      <c r="E31" s="7" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="12"/>
-      <c r="B32" s="9"/>
+      <c r="E31" s="15" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="11"/>
+      <c r="B32" s="8"/>
       <c r="C32" s="3" t="s">
         <v>53</v>
       </c>
@@ -1597,9 +1596,9 @@
         <v>98</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="12"/>
-      <c r="B33" s="9"/>
+    <row r="33" spans="1:7" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="11"/>
+      <c r="B33" s="8"/>
       <c r="C33" s="3" t="s">
         <v>56</v>
       </c>
@@ -1607,12 +1606,12 @@
         <v>99</v>
       </c>
       <c r="E33" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="12"/>
-      <c r="B34" s="9"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="11"/>
+      <c r="B34" s="8"/>
       <c r="C34" s="3" t="s">
         <v>57</v>
       </c>
@@ -1620,81 +1619,81 @@
         <v>57</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="13.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="13"/>
-      <c r="B35" s="10"/>
+    <row r="35" spans="1:7" ht="13.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A35" s="12"/>
+      <c r="B35" s="9"/>
       <c r="C35" s="4" t="s">
         <v>58</v>
       </c>
       <c r="D35" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E35" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="8" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="B36" s="8" t="s">
+      <c r="B36" s="7" t="s">
         <v>60</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D36" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E36" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="F36" t="s">
-        <v>104</v>
-      </c>
-      <c r="G36" s="7" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="9"/>
-      <c r="B37" s="9"/>
+        <v>105</v>
+      </c>
+      <c r="G36" s="15" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="8"/>
+      <c r="B37" s="8"/>
       <c r="C37" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D37" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="9"/>
-      <c r="B38" s="9"/>
+        <v>106</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="8"/>
+      <c r="B38" s="8"/>
       <c r="C38" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D38" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E38" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="9"/>
-      <c r="B39" s="9"/>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="8"/>
+      <c r="B39" s="8"/>
       <c r="C39" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D39" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E39" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" ht="13.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="10"/>
-      <c r="B40" s="10"/>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="13.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A40" s="9"/>
+      <c r="B40" s="9"/>
       <c r="C40" s="4" t="s">
         <v>4</v>
       </c>
@@ -1702,11 +1701,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="8" t="s">
+    <row r="41" spans="1:7" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="B41" s="8" t="s">
+      <c r="B41" s="7" t="s">
         <v>62</v>
       </c>
       <c r="C41" s="3" t="s">
@@ -1716,42 +1715,42 @@
         <v>5</v>
       </c>
       <c r="E41" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="9"/>
-      <c r="B42" s="9"/>
+        <v>111</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="8"/>
+      <c r="B42" s="8"/>
       <c r="C42" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D42" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="9"/>
-      <c r="B43" s="9"/>
+        <v>112</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="8"/>
+      <c r="B43" s="8"/>
       <c r="C43" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D43" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="9"/>
-      <c r="B44" s="9"/>
+        <v>113</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="8"/>
+      <c r="B44" s="8"/>
       <c r="C44" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D44" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" ht="13.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="10"/>
-      <c r="B45" s="10"/>
+        <v>114</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="13.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A45" s="9"/>
+      <c r="B45" s="9"/>
       <c r="C45" s="4" t="s">
         <v>9</v>
       </c>
@@ -1759,13 +1758,19 @@
         <v>9</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="5" t="s">
         <v>63</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="B2:B6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="B9:B11"/>
     <mergeCell ref="A41:A45"/>
     <mergeCell ref="B41:B45"/>
     <mergeCell ref="A29:A35"/>
@@ -1780,12 +1785,6 @@
     <mergeCell ref="B22:B26"/>
     <mergeCell ref="A27:A28"/>
     <mergeCell ref="B27:B28"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="B2:B6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="B9:B11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>